<commit_message>
Organized everything I have so far so it is all visible, added the plane, stopped the pyramid from rotating and moved it from outside the penguins feet.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -951,7 +954,7 @@
   <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +1709,9 @@
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
@@ -1731,7 +1736,9 @@
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="16">
         <f t="shared" si="0"/>
@@ -1756,7 +1763,9 @@
       <c r="D30" s="5">
         <v>1</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
@@ -1781,7 +1790,9 @@
       <c r="D31" s="5">
         <v>1</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="16">
         <f t="shared" ref="G31:G65" si="1" xml:space="preserve"> IF(EXACT(F31,"X"),IF(EXACT(E31,"I"),$B31,IF(EXACT(E31,"II"),$C31,IF(EXACT(E31,"III"),$D31,0))),0)</f>
@@ -1831,7 +1842,9 @@
       <c r="D33" s="5">
         <v>4</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
@@ -1856,7 +1869,9 @@
       <c r="D34" s="5">
         <v>4</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Begun work on the skybox, currently creating variables to prepare it for drawing, also moved the geometry shader penguin back inside of the real model due to moving with camera
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1261,9 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="16">
         <f xml:space="preserve"> IF(EXACT(F9,"X"),IF(EXACT(E9,"I"),$B9,IF(EXACT(E9,"II"),$C9,IF(EXACT(E9,"III"),$D9,0))),0)</f>
@@ -1519,7 +1521,9 @@
       <c r="D20" s="5">
         <v>3</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="16">
         <f t="shared" si="0"/>
@@ -1974,7 +1978,9 @@
       <c r="D39" s="5">
         <v>1</v>
       </c>
-      <c r="E39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F39" s="3"/>
       <c r="G39" s="16">
         <f t="shared" si="1"/>
@@ -3078,7 +3084,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Still working on Skybox and shaders, probably have enough for its pixel shader
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>III</t>
+  </si>
+  <si>
+    <t>http://richardssoftware.net/Home/Post/25</t>
   </si>
 </sst>
 </file>
@@ -953,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,11 +1097,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1151,15 +1154,11 @@
       <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84)  &gt; 18, SUMIF(E4:E81,"=I",G4:G81) + SUMIF(C83:C84, "X",B83:B84) - 18,0)</f>
@@ -1167,7 +1166,7 @@
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) - 18,0)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) - 18,0)</f>
@@ -1235,7 +1234,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -2994,7 +2993,9 @@
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
+      <c r="A88" s="12" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>

</xml_diff>

<commit_message>
Skybox works correctly, took out pyramid for testing purposes, need to put that back in.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -80,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="97">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -965,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,15 +1102,15 @@
       </c>
       <c r="J4" s="11">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K4" s="11">
         <f>SUM(H6,I6,J6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L4" s="11">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1176,7 +1175,7 @@
       </c>
       <c r="I6" s="11">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) - 18,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J6" s="11">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) - 18,0)</f>
@@ -1244,7 +1243,7 @@
       </c>
       <c r="H8" s="14">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I8" s="11">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -1252,7 +1251,7 @@
       </c>
       <c r="J8" s="11">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1533,10 +1532,12 @@
       <c r="E20" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="G20" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1725,10 +1726,12 @@
       <c r="E28" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="9"/>
+      <c r="F28" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="G28" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1855,9 +1858,7 @@
       <c r="D33" s="2">
         <v>4</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>95</v>
-      </c>
+      <c r="E33" s="8"/>
       <c r="F33" s="9"/>
       <c r="G33" s="10">
         <f t="shared" si="1"/>
@@ -3095,7 +3096,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Commented out everything I have so far for viewports, I got a second one on the other half of the screen, but does not yet render anything.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="97">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -964,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2574,7 +2574,9 @@
       <c r="D65" s="2">
         <v>4</v>
       </c>
-      <c r="E65" s="8"/>
+      <c r="E65" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="F65" s="9"/>
       <c r="G65" s="10">
         <f t="shared" si="1"/>
@@ -3096,7 +3098,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Switched plane to draw using the original vs and ps, now the plane is being lit, still no normal mapping though.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="99">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>http://richardssoftware.net/Home/Post/25</t>
+  </si>
+  <si>
+    <t>http://www.rastertek.com/dx11tut36.html</t>
+  </si>
+  <si>
+    <t>https://www.braynzarsoft.net</t>
   </si>
 </sst>
 </file>
@@ -555,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -622,6 +628,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -965,7 +974,7 @@
   <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1111,7 @@
       </c>
       <c r="J4" s="11">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K4" s="11">
         <f>SUM(H6,I6,J6)</f>
@@ -1110,7 +1119,7 @@
       </c>
       <c r="L4" s="11">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1251,7 +1260,7 @@
       </c>
       <c r="J8" s="11">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1269,9 +1278,7 @@
       <c r="D9" s="2">
         <v>1</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>95</v>
-      </c>
+      <c r="E9" s="8"/>
       <c r="F9" s="9"/>
       <c r="G9" s="10">
         <f xml:space="preserve"> IF(EXACT(F9,"X"),IF(EXACT(E9,"I"),$B9,IF(EXACT(E9,"II"),$C9,IF(EXACT(E9,"III"),$D9,0))),0)</f>
@@ -1752,9 +1759,7 @@
       <c r="D29" s="2">
         <v>1</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>95</v>
-      </c>
+      <c r="E29" s="8"/>
       <c r="F29" s="9"/>
       <c r="G29" s="10">
         <f t="shared" si="0"/>
@@ -1779,9 +1784,7 @@
       <c r="D30" s="2">
         <v>1</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>95</v>
-      </c>
+      <c r="E30" s="8"/>
       <c r="F30" s="9"/>
       <c r="G30" s="10">
         <f t="shared" si="0"/>
@@ -1806,9 +1809,7 @@
       <c r="D31" s="2">
         <v>1</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>95</v>
-      </c>
+      <c r="E31" s="8"/>
       <c r="F31" s="9"/>
       <c r="G31" s="10">
         <f t="shared" ref="G31:G65" si="1" xml:space="preserve"> IF(EXACT(F31,"X"),IF(EXACT(E31,"I"),$B31,IF(EXACT(E31,"II"),$C31,IF(EXACT(E31,"III"),$D31,0))),0)</f>
@@ -1988,9 +1989,7 @@
       <c r="D39" s="2">
         <v>1</v>
       </c>
-      <c r="E39" s="8" t="s">
-        <v>95</v>
-      </c>
+      <c r="E39" s="8"/>
       <c r="F39" s="9"/>
       <c r="G39" s="10">
         <f t="shared" si="1"/>
@@ -2321,7 +2320,9 @@
       <c r="D54" s="2">
         <v>2</v>
       </c>
-      <c r="E54" s="8"/>
+      <c r="E54" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="F54" s="9"/>
       <c r="G54" s="10">
         <f t="shared" si="1"/>
@@ -2577,10 +2578,12 @@
       <c r="E65" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F65" s="9"/>
+      <c r="F65" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="G65" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -2941,7 +2944,9 @@
       <c r="D83" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E83" s="9"/>
+      <c r="E83" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
@@ -2963,7 +2968,9 @@
       <c r="D84" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E84" s="9"/>
+      <c r="E84" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
@@ -3011,10 +3018,14 @@
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="21"/>
+      <c r="A89" s="21" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="21"/>
+      <c r="A90" s="23" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="21"/>
@@ -3098,7 +3109,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>